<commit_message>
1. Add store requisition and it's item. 2. Allow to add material during the process of the workorder. 3. Allow to update the particular material during the process of the workorder. 4. add 2 tables.
</commit_message>
<xml_diff>
--- a/db/project.xlsx
+++ b/db/project.xlsx
@@ -134,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B79" authorId="0">
+    <comment ref="B80" authorId="0">
       <text>
         <r>
           <rPr>
@@ -167,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B100" authorId="0">
+    <comment ref="B101" authorId="0">
       <text>
         <r>
           <rPr>
@@ -219,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B115" authorId="0">
+    <comment ref="B116" authorId="0">
       <text>
         <r>
           <rPr>
@@ -272,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C124" authorId="0">
+    <comment ref="C125" authorId="0">
       <text>
         <r>
           <rPr>
@@ -305,7 +305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C139" authorId="0">
+    <comment ref="C141" authorId="0">
       <text>
         <r>
           <rPr>
@@ -338,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B148" authorId="0">
+    <comment ref="B150" authorId="0">
       <text>
         <r>
           <rPr>
@@ -521,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C158" authorId="0">
+    <comment ref="C160" authorId="0">
       <text>
         <r>
           <rPr>
@@ -555,7 +555,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C159" authorId="0">
+    <comment ref="C161" authorId="0">
       <text>
         <r>
           <rPr>
@@ -588,7 +588,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B167" authorId="0">
+    <comment ref="B169" authorId="0">
       <text>
         <r>
           <rPr>
@@ -679,7 +679,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B181" authorId="0">
+    <comment ref="B183" authorId="0">
       <text>
         <r>
           <rPr>
@@ -755,7 +755,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="262">
   <si>
     <t>1）库存管理是需要的，制定计划是需要确认库存是否充足；</t>
   </si>
@@ -1710,10 +1710,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>工单表ID，=0说明不指定工单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>store_requisition_item</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1739,10 +1735,6 @@
   </si>
   <si>
     <t>signed_uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>created_time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1958,6 +1950,22 @@
   </si>
   <si>
     <t>工艺表子表ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tinyint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否有效，0-无效，1-有效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>created_date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2675,13 +2683,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G210"/>
+  <dimension ref="A2:G212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F87" sqref="F87"/>
+      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2911,7 +2919,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3262,7 +3270,7 @@
         <v>16</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -3292,146 +3300,147 @@
         <v>2</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="C48" s="7"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="E48" s="14">
+        <v>1</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8" t="s">
+      <c r="C49" s="7"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="B50" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="B51" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="B52" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C52" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D51" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E51" s="7">
-        <v>4</v>
-      </c>
-      <c r="F51" s="7" t="s">
+      <c r="D52" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" s="7">
+        <v>4</v>
+      </c>
+      <c r="F52" s="7" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="C52" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E52" s="7">
-        <v>16</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="C53" s="7" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>78</v>
       </c>
       <c r="E53" s="7">
+        <v>16</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="C54" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E54" s="7">
         <v>32</v>
       </c>
-      <c r="F53" s="7" t="s">
+      <c r="F54" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
-      <c r="C54" s="17" t="s">
+    <row r="55" spans="1:6">
+      <c r="C55" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D55" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="E54" s="17">
+      <c r="E55" s="17">
         <v>2</v>
       </c>
-      <c r="F54" s="17" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="B55" s="7" t="s">
-        <v>14</v>
+      <c r="F55" s="17" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="B56" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="B57" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C57" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E56" s="7">
-        <v>4</v>
-      </c>
-      <c r="F56" s="7" t="s">
+      <c r="E57" s="7">
+        <v>4</v>
+      </c>
+      <c r="F57" s="7" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="C57" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E57" s="7">
-        <v>16</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="C58" s="7" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>78</v>
       </c>
       <c r="E58" s="7">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>149</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="C59" s="7" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>78</v>
       </c>
       <c r="E59" s="7">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="C60" s="7" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>78</v>
@@ -3440,210 +3449,210 @@
         <v>16</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>242</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="C61" s="7" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>78</v>
       </c>
       <c r="E61" s="7">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="C62" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E62" s="7">
+        <v>2</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="C63" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D63" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E62" s="7">
+      <c r="E63" s="7">
         <v>1</v>
       </c>
-      <c r="F62" s="7" t="s">
+      <c r="F63" s="7" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="B63" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="B64" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6">
+      <c r="B65" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C65" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D64" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E64" s="7">
-        <v>4</v>
-      </c>
-      <c r="F64" s="7" t="s">
+      <c r="D65" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E65" s="7">
+        <v>4</v>
+      </c>
+      <c r="F65" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="2:6">
-      <c r="C65" s="8" t="s">
+    <row r="66" spans="2:6">
+      <c r="C66" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D65" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E65" s="7">
-        <v>4</v>
-      </c>
-      <c r="F65" s="7" t="s">
+      <c r="D66" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E66" s="7">
+        <v>4</v>
+      </c>
+      <c r="F66" s="7" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6">
-      <c r="C66" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D66" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E66" s="7">
-        <v>16</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="67" spans="2:6">
       <c r="C67" s="7" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D67" s="7" t="s">
         <v>78</v>
       </c>
       <c r="E67" s="7">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="2:6">
       <c r="C68" s="7" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E68" s="7">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>237</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="2:6">
       <c r="C69" s="7" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="E69" s="7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="2:6">
       <c r="C70" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E70" s="7">
+        <v>2</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6">
+      <c r="C71" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D71" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E70" s="7">
+      <c r="E71" s="7">
         <v>1</v>
       </c>
-      <c r="F70" s="7" t="s">
+      <c r="F71" s="7" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6">
-      <c r="B71" s="7" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="72" spans="2:6">
       <c r="B72" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="B73" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="C73" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D72" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E72" s="7">
-        <v>4</v>
-      </c>
-      <c r="F72" s="7" t="s">
+      <c r="D73" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E73" s="7">
+        <v>4</v>
+      </c>
+      <c r="F73" s="7" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6">
-      <c r="C73" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E73" s="7">
-        <v>4</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="74" spans="2:6">
       <c r="C74" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E74" s="7">
+        <v>4</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6">
+      <c r="C75" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D74" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E74" s="7">
-        <v>4</v>
-      </c>
-      <c r="F74" s="7" t="s">
+      <c r="D75" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E75" s="7">
+        <v>4</v>
+      </c>
+      <c r="F75" s="7" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6">
-      <c r="C75" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E75" s="7">
-        <v>8</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="76" spans="2:6">
       <c r="C76" s="7" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>102</v>
@@ -3652,65 +3661,65 @@
         <v>8</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>152</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="2:6">
       <c r="C77" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E77" s="7">
+        <v>8</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6">
+      <c r="C78" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D78" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E77" s="7">
+      <c r="E78" s="7">
         <v>2</v>
       </c>
-      <c r="F77" s="7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6">
-      <c r="B78" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C78" s="9"/>
-      <c r="D78" s="10"/>
-      <c r="F78" s="10"/>
+      <c r="F78" s="7" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="79" spans="2:6">
       <c r="B79" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C79" s="9"/>
+      <c r="D79" s="10"/>
+      <c r="F79" s="10"/>
+    </row>
+    <row r="80" spans="2:6">
+      <c r="B80" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C79" s="9" t="s">
+      <c r="C80" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D79" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E79" s="7">
-        <v>4</v>
-      </c>
-      <c r="F79" s="7" t="s">
+      <c r="D80" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E80" s="7">
+        <v>4</v>
+      </c>
+      <c r="F80" s="7" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6">
-      <c r="C80" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E80" s="7">
-        <v>4</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="81" spans="2:6">
       <c r="C81" s="9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>67</v>
@@ -3719,88 +3728,88 @@
         <v>4</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" spans="2:6">
       <c r="C82" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E82" s="7">
+        <v>4</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6">
+      <c r="C83" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D82" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E82" s="7">
-        <v>4</v>
-      </c>
-      <c r="F82" s="7" t="s">
+      <c r="D83" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E83" s="7">
+        <v>4</v>
+      </c>
+      <c r="F83" s="7" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6">
-      <c r="C83" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E83" s="7">
-        <v>16</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="84" spans="2:6">
       <c r="C84" s="7" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E84" s="7">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
     </row>
     <row r="85" spans="2:6">
       <c r="C85" s="7" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>68</v>
       </c>
+      <c r="E85" s="7">
+        <v>1</v>
+      </c>
       <c r="F85" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6">
+      <c r="C86" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F86" s="7" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6">
-      <c r="B86" s="7" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="87" spans="2:6">
       <c r="B87" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6">
+      <c r="B88" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C87" s="8" t="s">
+      <c r="C88" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D87" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E87" s="7">
-        <v>4</v>
-      </c>
-      <c r="F87" s="7" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6">
-      <c r="C88" s="9" t="s">
-        <v>72</v>
-      </c>
       <c r="D88" s="7" t="s">
         <v>67</v>
       </c>
@@ -3808,12 +3817,12 @@
         <v>4</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>60</v>
+        <v>257</v>
       </c>
     </row>
     <row r="89" spans="2:6">
       <c r="C89" s="9" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>67</v>
@@ -3822,12 +3831,12 @@
         <v>4</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="90" spans="2:6">
       <c r="C90" s="9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D90" s="7" t="s">
         <v>67</v>
@@ -3836,54 +3845,54 @@
         <v>4</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
     </row>
     <row r="91" spans="2:6">
       <c r="C91" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E91" s="7">
+        <v>4</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6">
+      <c r="C92" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D91" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E91" s="7">
-        <v>4</v>
-      </c>
-      <c r="F91" s="7" t="s">
+      <c r="D92" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E92" s="7">
+        <v>4</v>
+      </c>
+      <c r="F92" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="92" spans="2:6">
-      <c r="C92" s="8" t="s">
+    <row r="93" spans="2:6">
+      <c r="C93" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D92" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E92" s="7">
-        <v>4</v>
-      </c>
-      <c r="F92" s="7" t="s">
+      <c r="D93" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E93" s="7">
+        <v>4</v>
+      </c>
+      <c r="F93" s="7" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="93" spans="2:6">
-      <c r="C93" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="E93" s="7">
-        <v>2</v>
-      </c>
-      <c r="F93" s="7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="94" spans="2:6">
       <c r="C94" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>110</v>
@@ -3892,26 +3901,26 @@
         <v>2</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
     </row>
     <row r="95" spans="2:6">
       <c r="C95" s="7" t="s">
-        <v>145</v>
+        <v>63</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="E95" s="7">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>147</v>
+        <v>104</v>
       </c>
     </row>
     <row r="96" spans="2:6">
       <c r="C96" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D96" s="7" t="s">
         <v>78</v>
@@ -3920,40 +3929,40 @@
         <v>16</v>
       </c>
       <c r="F96" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6">
+      <c r="C97" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E97" s="7">
+        <v>16</v>
+      </c>
+      <c r="F97" s="7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="98" spans="2:6">
-      <c r="B98" s="8" t="s">
+    <row r="99" spans="2:6">
+      <c r="B99" s="8" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="99" spans="2:6">
-      <c r="B99" s="7" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="100" spans="2:6">
       <c r="B100" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6">
+      <c r="B101" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C100" s="8" t="s">
+      <c r="C101" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D100" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E100" s="7">
-        <v>4</v>
-      </c>
-      <c r="F100" s="7" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6">
-      <c r="C101" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="D101" s="7" t="s">
         <v>67</v>
       </c>
@@ -3961,12 +3970,12 @@
         <v>4</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>107</v>
+        <v>243</v>
       </c>
     </row>
     <row r="102" spans="2:6">
       <c r="C102" s="9" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>67</v>
@@ -3975,12 +3984,12 @@
         <v>4</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
     </row>
     <row r="103" spans="2:6">
       <c r="C103" s="9" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D103" s="7" t="s">
         <v>67</v>
@@ -3989,82 +3998,82 @@
         <v>4</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>189</v>
+        <v>38</v>
       </c>
     </row>
     <row r="104" spans="2:6">
       <c r="C104" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E104" s="7">
+        <v>4</v>
+      </c>
+      <c r="F104" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6">
+      <c r="C105" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D104" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E104" s="7">
-        <v>4</v>
-      </c>
-      <c r="F104" s="7" t="s">
+      <c r="D105" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E105" s="7">
+        <v>4</v>
+      </c>
+      <c r="F105" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="105" spans="2:6">
-      <c r="C105" s="8" t="s">
+    <row r="106" spans="2:6">
+      <c r="C106" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D105" s="7" t="s">
+      <c r="D106" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E105" s="7">
+      <c r="E106" s="7">
         <v>16</v>
       </c>
-      <c r="F105" s="7" t="s">
+      <c r="F106" s="7" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="106" spans="2:6">
-      <c r="C106" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E106" s="7">
-        <v>8</v>
-      </c>
-      <c r="F106" s="7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="107" spans="2:6">
       <c r="C107" s="7" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="E107" s="7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>239</v>
+        <v>34</v>
       </c>
     </row>
     <row r="108" spans="2:6">
       <c r="C108" s="7" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="D108" s="7" t="s">
-        <v>200</v>
+        <v>78</v>
       </c>
       <c r="E108" s="7">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>86</v>
+        <v>237</v>
       </c>
     </row>
     <row r="109" spans="2:6">
       <c r="C109" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D109" s="7" t="s">
         <v>200</v>
@@ -4073,12 +4082,12 @@
         <v>8</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="110" spans="2:6">
       <c r="C110" s="7" t="s">
-        <v>159</v>
+        <v>89</v>
       </c>
       <c r="D110" s="7" t="s">
         <v>200</v>
@@ -4087,146 +4096,146 @@
         <v>8</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="111" spans="2:6">
       <c r="C111" s="7" t="s">
-        <v>82</v>
+        <v>159</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>67</v>
+        <v>200</v>
       </c>
       <c r="E111" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F111" s="7" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112" spans="2:6">
       <c r="C112" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>200</v>
+        <v>67</v>
       </c>
       <c r="E112" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F112" s="7" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
     <row r="113" spans="2:6">
       <c r="C113" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E113" s="7">
+        <v>8</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6">
+      <c r="C114" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D113" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E113" s="7">
-        <v>4</v>
-      </c>
-      <c r="F113" s="7" t="s">
+      <c r="D114" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E114" s="7">
+        <v>4</v>
+      </c>
+      <c r="F114" s="7" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="114" spans="2:6">
-      <c r="B114" s="7" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="115" spans="2:6">
       <c r="B115" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6">
+      <c r="B116" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C115" s="8" t="s">
+      <c r="C116" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D115" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E115" s="7">
-        <v>4</v>
-      </c>
-      <c r="F115" s="7" t="s">
+      <c r="D116" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E116" s="7">
+        <v>4</v>
+      </c>
+      <c r="F116" s="7" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="116" spans="2:6">
-      <c r="C116" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D116" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E116" s="7">
-        <v>4</v>
-      </c>
-      <c r="F116" s="7" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="117" spans="2:6">
       <c r="C117" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D117" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E117" s="7">
+        <v>4</v>
+      </c>
+      <c r="F117" s="7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="118" spans="2:6">
+      <c r="C118" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D117" s="7" t="s">
+      <c r="D118" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E117" s="7">
+      <c r="E118" s="7">
         <v>2</v>
       </c>
-      <c r="F117" s="7" t="s">
+      <c r="F118" s="7" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="118" spans="2:6">
-      <c r="C118" s="9" t="s">
+    <row r="119" spans="2:6">
+      <c r="C119" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D118" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E118" s="7">
-        <v>4</v>
-      </c>
-      <c r="F118" s="7" t="s">
+      <c r="D119" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E119" s="7">
+        <v>4</v>
+      </c>
+      <c r="F119" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="119" spans="2:6">
-      <c r="C119" s="15" t="s">
+    <row r="120" spans="2:6">
+      <c r="C120" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D119" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E119" s="14">
-        <v>4</v>
-      </c>
-      <c r="F119" s="14" t="s">
+      <c r="D120" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E120" s="14">
+        <v>4</v>
+      </c>
+      <c r="F120" s="14" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="120" spans="2:6">
-      <c r="C120" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D120" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E120" s="7">
-        <v>4</v>
-      </c>
-      <c r="F120" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="121" spans="2:6">
       <c r="C121" s="9" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D121" s="7" t="s">
         <v>67</v>
@@ -4235,82 +4244,82 @@
         <v>4</v>
       </c>
       <c r="F121" s="7" t="s">
-        <v>189</v>
+        <v>38</v>
       </c>
     </row>
     <row r="122" spans="2:6">
       <c r="C122" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D122" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E122" s="7">
+        <v>4</v>
+      </c>
+      <c r="F122" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="123" spans="2:6">
+      <c r="C123" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D122" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E122" s="7">
-        <v>4</v>
-      </c>
-      <c r="F122" s="7" t="s">
+      <c r="D123" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E123" s="7">
+        <v>4</v>
+      </c>
+      <c r="F123" s="7" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6">
-      <c r="C123" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D123" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E123" s="7">
-        <v>16</v>
-      </c>
-      <c r="F123" s="7" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="124" spans="2:6">
       <c r="C124" s="7" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E124" s="7">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F124" s="7" t="s">
-        <v>153</v>
+        <v>80</v>
       </c>
     </row>
     <row r="125" spans="2:6">
       <c r="C125" s="7" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="E125" s="7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F125" s="7" t="s">
-        <v>239</v>
+        <v>153</v>
       </c>
     </row>
     <row r="126" spans="2:6">
       <c r="C126" s="7" t="s">
-        <v>123</v>
+        <v>13</v>
       </c>
       <c r="D126" s="7" t="s">
-        <v>200</v>
+        <v>78</v>
       </c>
       <c r="E126" s="7">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F126" s="7" t="s">
-        <v>125</v>
+        <v>237</v>
       </c>
     </row>
     <row r="127" spans="2:6">
       <c r="C127" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D127" s="7" t="s">
         <v>200</v>
@@ -4319,40 +4328,40 @@
         <v>8</v>
       </c>
       <c r="F127" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="128" spans="2:6">
       <c r="C128" s="7" t="s">
-        <v>41</v>
+        <v>124</v>
       </c>
       <c r="D128" s="7" t="s">
-        <v>68</v>
+        <v>200</v>
       </c>
       <c r="E128" s="7">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F128" s="7" t="s">
-        <v>190</v>
+        <v>126</v>
       </c>
     </row>
     <row r="129" spans="2:6">
       <c r="C129" s="7" t="s">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="D129" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E129" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F129" s="7" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
     </row>
     <row r="130" spans="2:6">
       <c r="C130" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D130" s="7" t="s">
         <v>67</v>
@@ -4361,146 +4370,146 @@
         <v>4</v>
       </c>
       <c r="F130" s="7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="131" spans="2:6">
       <c r="C131" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D131" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E131" s="7">
+        <v>4</v>
+      </c>
+      <c r="F131" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6">
+      <c r="C132" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D131" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E131" s="7">
-        <v>4</v>
-      </c>
-      <c r="F131" s="7" t="s">
+      <c r="D132" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E132" s="7">
+        <v>4</v>
+      </c>
+      <c r="F132" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="132" spans="2:6">
-      <c r="B132" s="7" t="s">
+    <row r="133" spans="2:6">
+      <c r="B133" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="133" spans="2:6">
-      <c r="B133" s="13" t="s">
+    <row r="134" spans="2:6">
+      <c r="B134" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="C133" s="8" t="s">
+      <c r="C134" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D133" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E133" s="7">
-        <v>4</v>
-      </c>
-      <c r="F133" s="7" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="134" spans="2:6">
-      <c r="C134" s="16" t="s">
+      <c r="D134" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E134" s="7">
+        <v>4</v>
+      </c>
+      <c r="F134" s="7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="135" spans="2:6">
+      <c r="C135" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D134" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E134" s="14">
-        <v>4</v>
-      </c>
-      <c r="F134" s="14" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="135" spans="2:6">
-      <c r="C135" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="D135" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E135" s="7">
-        <v>4</v>
-      </c>
-      <c r="F135" s="7" t="s">
-        <v>161</v>
+      <c r="D135" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E135" s="14">
+        <v>4</v>
+      </c>
+      <c r="F135" s="14" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="136" spans="2:6">
       <c r="C136" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D136" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E136" s="7">
+        <v>4</v>
+      </c>
+      <c r="F136" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6">
+      <c r="C137" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D136" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E136" s="7">
-        <v>4</v>
-      </c>
-      <c r="F136" s="7" t="s">
+      <c r="D137" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E137" s="7">
+        <v>4</v>
+      </c>
+      <c r="F137" s="7" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="137" spans="2:6">
-      <c r="C137" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D137" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E137" s="14">
-        <v>4</v>
-      </c>
-      <c r="F137" s="14" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="138" spans="2:6">
       <c r="C138" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D138" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E138" s="14">
+        <v>4</v>
+      </c>
+      <c r="F138" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="139" spans="2:6">
+      <c r="C139" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D139" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E139" s="14">
+        <v>4</v>
+      </c>
+      <c r="F139" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="140" spans="2:6">
+      <c r="C140" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D138" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E138" s="14">
-        <v>4</v>
-      </c>
-      <c r="F138" s="14" t="s">
+      <c r="D140" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E140" s="14">
+        <v>4</v>
+      </c>
+      <c r="F140" s="14" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="139" spans="2:6">
-      <c r="C139" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D139" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E139" s="7">
-        <v>8</v>
-      </c>
-      <c r="F139" s="7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="140" spans="2:6">
-      <c r="C140" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D140" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E140" s="7">
-        <v>8</v>
-      </c>
-      <c r="F140" s="7" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="141" spans="2:6">
       <c r="C141" s="7" t="s">
-        <v>202</v>
+        <v>77</v>
       </c>
       <c r="D141" s="7" t="s">
         <v>102</v>
@@ -4509,12 +4518,12 @@
         <v>8</v>
       </c>
       <c r="F141" s="7" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="142" spans="2:6">
       <c r="C142" s="7" t="s">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="D142" s="7" t="s">
         <v>102</v>
@@ -4523,177 +4532,177 @@
         <v>8</v>
       </c>
       <c r="F142" s="7" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
     </row>
     <row r="143" spans="2:6">
       <c r="C143" s="7" t="s">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="D143" s="7" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="E143" s="7">
         <v>8</v>
       </c>
       <c r="F143" s="7" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="144" spans="2:6">
       <c r="C144" s="7" t="s">
-        <v>13</v>
+        <v>191</v>
       </c>
       <c r="D144" s="7" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="E144" s="7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F144" s="7" t="s">
-        <v>238</v>
+        <v>193</v>
       </c>
     </row>
     <row r="145" spans="2:6">
       <c r="C145" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D145" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E145" s="7">
+        <v>8</v>
+      </c>
+      <c r="F145" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="146" spans="2:6">
+      <c r="C146" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D146" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E146" s="7">
+        <v>2</v>
+      </c>
+      <c r="F146" s="7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="147" spans="2:6">
+      <c r="C147" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D145" s="7" t="s">
+      <c r="D147" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E145" s="7">
+      <c r="E147" s="7">
         <v>1</v>
       </c>
-      <c r="F145" s="7" t="s">
+      <c r="F147" s="7" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="146" spans="2:6">
-      <c r="C146" s="14" t="s">
+    <row r="148" spans="2:6">
+      <c r="C148" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D148" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E148" s="14">
+        <v>1</v>
+      </c>
+      <c r="F148" s="14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="149" spans="2:6">
+      <c r="C149" s="7"/>
+    </row>
+    <row r="150" spans="2:6">
+      <c r="B150" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="151" spans="2:6">
+      <c r="B151" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C151" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D151" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E151" s="7">
+        <v>4</v>
+      </c>
+      <c r="F151" s="7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="152" spans="2:6">
+      <c r="C152" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D152" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E152" s="14">
+        <v>4</v>
+      </c>
+      <c r="F152" s="14" t="s">
         <v>247</v>
-      </c>
-      <c r="D146" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E146" s="14">
-        <v>1</v>
-      </c>
-      <c r="F146" s="14" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="147" spans="2:6">
-      <c r="C147" s="7"/>
-    </row>
-    <row r="148" spans="2:6">
-      <c r="B148" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="149" spans="2:6">
-      <c r="B149" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C149" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D149" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E149" s="7">
-        <v>4</v>
-      </c>
-      <c r="F149" s="7" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="150" spans="2:6">
-      <c r="C150" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D150" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E150" s="14">
-        <v>4</v>
-      </c>
-      <c r="F150" s="14" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="151" spans="2:6">
-      <c r="C151" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="D151" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E151" s="7">
-        <v>4</v>
-      </c>
-      <c r="F151" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="152" spans="2:6">
-      <c r="C152" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D152" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E152" s="7">
-        <v>4</v>
-      </c>
-      <c r="F152" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="153" spans="2:6">
       <c r="C153" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D153" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E153" s="7">
+        <v>4</v>
+      </c>
+      <c r="F153" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="154" spans="2:6">
+      <c r="C154" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D154" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E154" s="7">
+        <v>4</v>
+      </c>
+      <c r="F154" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="155" spans="2:6">
+      <c r="C155" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D153" s="7" t="s">
+      <c r="D155" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E153" s="7">
+      <c r="E155" s="7">
         <v>2</v>
       </c>
-      <c r="F153" s="7" t="s">
+      <c r="F155" s="7" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="154" spans="2:6">
-      <c r="C154" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D154" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E154" s="7">
-        <v>4</v>
-      </c>
-      <c r="F154" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="155" spans="2:6">
-      <c r="C155" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D155" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E155" s="7">
-        <v>4</v>
-      </c>
-      <c r="F155" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="156" spans="2:6">
       <c r="C156" s="9" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D156" s="7" t="s">
         <v>67</v>
@@ -4702,12 +4711,12 @@
         <v>4</v>
       </c>
       <c r="F156" s="7" t="s">
-        <v>37</v>
+        <v>107</v>
       </c>
     </row>
     <row r="157" spans="2:6">
       <c r="C157" s="9" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="D157" s="7" t="s">
         <v>67</v>
@@ -4716,12 +4725,12 @@
         <v>4</v>
       </c>
       <c r="F157" s="7" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
     </row>
     <row r="158" spans="2:6">
       <c r="C158" s="9" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="D158" s="7" t="s">
         <v>67</v>
@@ -4730,532 +4739,530 @@
         <v>4</v>
       </c>
       <c r="F158" s="7" t="s">
-        <v>166</v>
+        <v>37</v>
       </c>
     </row>
     <row r="159" spans="2:6">
       <c r="C159" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D159" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E159" s="7">
+        <v>4</v>
+      </c>
+      <c r="F159" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="160" spans="2:6">
+      <c r="C160" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D160" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E160" s="7">
+        <v>4</v>
+      </c>
+      <c r="F160" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="161" spans="2:6">
+      <c r="C161" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="D159" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E159" s="7">
-        <v>4</v>
-      </c>
-      <c r="F159" s="7" t="s">
+      <c r="D161" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E161" s="7">
+        <v>4</v>
+      </c>
+      <c r="F161" s="7" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="160" spans="2:6">
-      <c r="C160" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="D160" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E160" s="7">
-        <v>8</v>
-      </c>
-      <c r="F160" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="161" spans="2:6">
-      <c r="C161" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D161" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E161" s="7">
-        <v>8</v>
-      </c>
-      <c r="F161" s="7" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="162" spans="2:6">
       <c r="C162" s="7" t="s">
-        <v>13</v>
+        <v>162</v>
       </c>
       <c r="D162" s="7" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="E162" s="7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F162" s="7" t="s">
-        <v>238</v>
+        <v>169</v>
       </c>
     </row>
     <row r="163" spans="2:6">
       <c r="C163" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D163" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E163" s="7">
+        <v>8</v>
+      </c>
+      <c r="F163" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="164" spans="2:6">
+      <c r="C164" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D164" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E164" s="7">
+        <v>2</v>
+      </c>
+      <c r="F164" s="7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="165" spans="2:6">
+      <c r="C165" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D163" s="7" t="s">
+      <c r="D165" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E163" s="7">
+      <c r="E165" s="7">
         <v>1</v>
       </c>
-      <c r="F163" s="7" t="s">
+      <c r="F165" s="7" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="164" spans="2:6">
-      <c r="C164" s="14" t="s">
+    <row r="166" spans="2:6">
+      <c r="C166" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D166" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E166" s="14">
+        <v>1</v>
+      </c>
+      <c r="F166" s="14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="167" spans="2:6">
+      <c r="C167" s="7"/>
+    </row>
+    <row r="168" spans="2:6">
+      <c r="B168" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="169" spans="2:6">
+      <c r="B169" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C169" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D169" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E169" s="7">
+        <v>4</v>
+      </c>
+      <c r="F169" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="170" spans="2:6">
+      <c r="C170" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D170" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E170" s="14">
+        <v>4</v>
+      </c>
+      <c r="F170" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="D164" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E164" s="14">
-        <v>1</v>
-      </c>
-      <c r="F164" s="14" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="165" spans="2:6">
-      <c r="C165" s="7"/>
-    </row>
-    <row r="166" spans="2:6">
-      <c r="B166" s="7" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="167" spans="2:6">
-      <c r="B167" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="C167" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D167" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E167" s="7">
-        <v>4</v>
-      </c>
-      <c r="F167" s="7" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="168" spans="2:6">
-      <c r="C168" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D168" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E168" s="14">
-        <v>4</v>
-      </c>
-      <c r="F168" s="14" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="169" spans="2:6">
-      <c r="C169" s="9" t="s">
+    </row>
+    <row r="171" spans="2:6">
+      <c r="C171" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="D169" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E169" s="7">
-        <v>4</v>
-      </c>
-      <c r="F169" s="7" t="s">
+      <c r="D171" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E171" s="7">
+        <v>4</v>
+      </c>
+      <c r="F171" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="170" spans="2:6">
-      <c r="C170" s="9" t="s">
+    <row r="172" spans="2:6">
+      <c r="C172" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D170" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E170" s="7">
-        <v>4</v>
-      </c>
-      <c r="F170" s="7" t="s">
+      <c r="D172" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E172" s="7">
+        <v>4</v>
+      </c>
+      <c r="F172" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="171" spans="2:6">
-      <c r="C171" s="8" t="s">
+    <row r="173" spans="2:6">
+      <c r="C173" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D171" s="7" t="s">
+      <c r="D173" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E171" s="7">
+      <c r="E173" s="7">
         <v>2</v>
       </c>
-      <c r="F171" s="7" t="s">
+      <c r="F173" s="7" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="172" spans="2:6">
-      <c r="C172" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D172" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E172" s="14">
-        <v>4</v>
-      </c>
-      <c r="F172" s="14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="173" spans="2:6">
-      <c r="C173" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D173" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E173" s="14">
-        <v>4</v>
-      </c>
-      <c r="F173" s="14" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="174" spans="2:6">
       <c r="C174" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D174" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E174" s="14">
+        <v>4</v>
+      </c>
+      <c r="F174" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="175" spans="2:6">
+      <c r="C175" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D175" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E175" s="14">
+        <v>4</v>
+      </c>
+      <c r="F175" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="176" spans="2:6">
+      <c r="C176" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D174" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E174" s="14">
-        <v>4</v>
-      </c>
-      <c r="F174" s="14" t="s">
+      <c r="D176" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E176" s="14">
+        <v>4</v>
+      </c>
+      <c r="F176" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="175" spans="2:6">
-      <c r="C175" s="9" t="s">
+    <row r="177" spans="2:7">
+      <c r="C177" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="D175" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E175" s="7">
-        <v>4</v>
-      </c>
-      <c r="F175" s="7" t="s">
+      <c r="D177" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E177" s="7">
+        <v>4</v>
+      </c>
+      <c r="F177" s="7" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="176" spans="2:6">
-      <c r="C176" s="9" t="s">
+    <row r="178" spans="2:7">
+      <c r="C178" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D176" s="7" t="s">
+      <c r="D178" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E176" s="7">
+      <c r="E178" s="7">
         <v>1</v>
       </c>
-      <c r="F176" s="7" t="s">
+      <c r="F178" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="177" spans="2:7">
-      <c r="C177" s="7" t="s">
+    <row r="179" spans="2:7">
+      <c r="C179" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D177" s="7" t="s">
+      <c r="D179" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="E177" s="7">
+      <c r="E179" s="7">
         <v>8</v>
       </c>
-      <c r="F177" s="7" t="s">
+      <c r="F179" s="7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="178" spans="2:7">
-      <c r="C178" s="7" t="s">
+    <row r="180" spans="2:7">
+      <c r="C180" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D178" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E178" s="7">
-        <v>4</v>
-      </c>
-      <c r="F178" s="7" t="s">
+      <c r="D180" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E180" s="7">
+        <v>4</v>
+      </c>
+      <c r="F180" s="7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="179" spans="2:7">
-      <c r="C179" s="7"/>
-    </row>
-    <row r="180" spans="2:7">
-      <c r="C180" s="7"/>
-    </row>
     <row r="181" spans="2:7">
-      <c r="B181" s="7" t="s">
+      <c r="C181" s="7"/>
+    </row>
+    <row r="182" spans="2:7">
+      <c r="C182" s="7"/>
+    </row>
+    <row r="183" spans="2:7">
+      <c r="B183" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="G183" s="11"/>
+    </row>
+    <row r="184" spans="2:7">
+      <c r="B184" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C184" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D184" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E184" s="7">
+        <v>4</v>
+      </c>
+      <c r="F184" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="185" spans="2:7">
+      <c r="C185" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D185" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E185" s="7">
+        <v>4</v>
+      </c>
+      <c r="F185" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="186" spans="2:7">
+      <c r="C186" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D186" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E186" s="7">
+        <v>4</v>
+      </c>
+      <c r="F186" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="187" spans="2:7">
+      <c r="C187" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="D187" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E187" s="14">
+        <v>4</v>
+      </c>
+      <c r="F187" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="G181" s="11"/>
-    </row>
-    <row r="182" spans="2:7">
-      <c r="B182" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="C182" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D182" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E182" s="7">
-        <v>4</v>
-      </c>
-      <c r="F182" s="7" t="s">
+    </row>
+    <row r="188" spans="2:7">
+      <c r="C188" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="D188" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E188" s="14">
+        <v>4</v>
+      </c>
+      <c r="F188" s="14" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="183" spans="2:7">
-      <c r="C183" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="D183" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E183" s="7">
-        <v>4</v>
-      </c>
-      <c r="F183" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="184" spans="2:7">
-      <c r="C184" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D184" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E184" s="7">
-        <v>4</v>
-      </c>
-      <c r="F184" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="185" spans="2:7">
-      <c r="C185" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="D185" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E185" s="14">
-        <v>4</v>
-      </c>
-      <c r="F185" s="14" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="186" spans="2:7">
-      <c r="C186" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="D186" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E186" s="14">
-        <v>4</v>
-      </c>
-      <c r="F186" s="14" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="187" spans="2:7">
-      <c r="C187" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D187" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E187" s="7">
-        <v>32</v>
-      </c>
-      <c r="F187" s="7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="188" spans="2:7">
-      <c r="C188" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D188" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E188" s="7">
-        <v>8</v>
-      </c>
-      <c r="F188" s="7" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="189" spans="2:7">
       <c r="C189" s="7" t="s">
-        <v>13</v>
+        <v>179</v>
       </c>
       <c r="D189" s="7" t="s">
         <v>78</v>
       </c>
       <c r="E189" s="7">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F189" s="7" t="s">
-        <v>239</v>
+        <v>180</v>
       </c>
     </row>
     <row r="190" spans="2:7">
       <c r="C190" s="7" t="s">
-        <v>182</v>
+        <v>77</v>
       </c>
       <c r="D190" s="7" t="s">
-        <v>200</v>
+        <v>102</v>
       </c>
       <c r="E190" s="7">
         <v>8</v>
       </c>
       <c r="F190" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="191" spans="2:7">
       <c r="C191" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D191" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E191" s="7">
+        <v>2</v>
+      </c>
+      <c r="F191" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="192" spans="2:7">
+      <c r="C192" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D192" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E192" s="7">
+        <v>8</v>
+      </c>
+      <c r="F192" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="193" spans="2:6">
+      <c r="C193" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D191" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E191" s="7">
-        <v>4</v>
-      </c>
-      <c r="F191" s="7" t="s">
+      <c r="D193" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E193" s="7">
+        <v>4</v>
+      </c>
+      <c r="F193" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="193" spans="2:6">
-      <c r="B193" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="C193" s="16"/>
-      <c r="D193" s="14"/>
-      <c r="E193" s="14"/>
-      <c r="F193" s="14"/>
-    </row>
-    <row r="194" spans="2:6">
-      <c r="B194" s="14" t="s">
+    <row r="195" spans="2:6">
+      <c r="B195" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="C195" s="16"/>
+      <c r="D195" s="14"/>
+      <c r="E195" s="14"/>
+      <c r="F195" s="14"/>
+    </row>
+    <row r="196" spans="2:6">
+      <c r="B196" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="C194" s="16" t="s">
+      <c r="C196" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="D194" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E194" s="14">
-        <v>4</v>
-      </c>
-      <c r="F194" s="14" t="s">
+      <c r="D196" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E196" s="14">
+        <v>4</v>
+      </c>
+      <c r="F196" s="14" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="195" spans="2:6">
-      <c r="B195" s="14"/>
-      <c r="C195" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="D195" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E195" s="14">
-        <v>4</v>
-      </c>
-      <c r="F195" s="14" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="196" spans="2:6">
-      <c r="B196" s="14"/>
-      <c r="C196" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="D196" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E196" s="14">
-        <v>4</v>
-      </c>
-      <c r="F196" s="14" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="197" spans="2:6">
       <c r="B197" s="14"/>
-      <c r="C197" s="14" t="s">
-        <v>56</v>
+      <c r="C197" s="16" t="s">
+        <v>219</v>
       </c>
       <c r="D197" s="14" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E197" s="14">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F197" s="14" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
     </row>
     <row r="198" spans="2:6">
       <c r="B198" s="14"/>
-      <c r="C198" s="14" t="s">
-        <v>231</v>
+      <c r="C198" s="16" t="s">
+        <v>220</v>
       </c>
       <c r="D198" s="14" t="s">
-        <v>200</v>
+        <v>67</v>
       </c>
       <c r="E198" s="14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F198" s="14" t="s">
-        <v>233</v>
+        <v>251</v>
       </c>
     </row>
     <row r="199" spans="2:6">
       <c r="B199" s="14"/>
       <c r="C199" s="14" t="s">
-        <v>174</v>
+        <v>56</v>
       </c>
       <c r="D199" s="14" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E199" s="14">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="F199" s="14" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
     </row>
     <row r="200" spans="2:6">
       <c r="B200" s="14"/>
       <c r="C200" s="14" t="s">
-        <v>182</v>
+        <v>261</v>
       </c>
       <c r="D200" s="14" t="s">
         <v>200</v>
@@ -5264,66 +5271,66 @@
         <v>8</v>
       </c>
       <c r="F200" s="14" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="201" spans="2:6">
       <c r="B201" s="14"/>
       <c r="C201" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D201" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E201" s="14">
+        <v>4</v>
+      </c>
+      <c r="F201" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="D201" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E201" s="14">
-        <v>4</v>
-      </c>
-      <c r="F201" s="14" t="s">
-        <v>235</v>
+    </row>
+    <row r="202" spans="2:6">
+      <c r="B202" s="14"/>
+      <c r="C202" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="D202" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E202" s="14">
+        <v>8</v>
+      </c>
+      <c r="F202" s="14" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="203" spans="2:6">
-      <c r="B203" s="14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="204" spans="2:6">
-      <c r="B204" s="14" t="s">
+      <c r="B203" s="14"/>
+      <c r="C203" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="D203" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E203" s="14">
+        <v>4</v>
+      </c>
+      <c r="F203" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="205" spans="2:6">
+      <c r="B205" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="C204" s="16" t="s">
+    </row>
+    <row r="206" spans="2:6">
+      <c r="B206" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="C206" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="D204" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E204" s="14">
-        <v>4</v>
-      </c>
-      <c r="F204" s="14" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="205" spans="2:6">
-      <c r="B205" s="14"/>
-      <c r="C205" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="D205" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E205" s="14">
-        <v>4</v>
-      </c>
-      <c r="F205" s="14" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="206" spans="2:6">
-      <c r="B206" s="14"/>
-      <c r="C206" s="16" t="s">
-        <v>219</v>
-      </c>
       <c r="D206" s="14" t="s">
         <v>67</v>
       </c>
@@ -5331,13 +5338,13 @@
         <v>4</v>
       </c>
       <c r="F206" s="14" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
     </row>
     <row r="207" spans="2:6">
       <c r="B207" s="14"/>
       <c r="C207" s="16" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D207" s="14" t="s">
         <v>67</v>
@@ -5346,50 +5353,80 @@
         <v>4</v>
       </c>
       <c r="F207" s="14" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="208" spans="2:6">
       <c r="B208" s="14"/>
-      <c r="C208" s="14" t="s">
+      <c r="C208" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="D208" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E208" s="14">
+        <v>4</v>
+      </c>
+      <c r="F208" s="14" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="209" spans="2:6">
+      <c r="B209" s="14"/>
+      <c r="C209" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="D209" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E209" s="14">
+        <v>4</v>
+      </c>
+      <c r="F209" s="14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="210" spans="2:6">
+      <c r="B210" s="14"/>
+      <c r="C210" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D208" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E208" s="14">
-        <v>4</v>
-      </c>
-      <c r="F208" s="14" t="s">
+      <c r="D210" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E210" s="14">
+        <v>4</v>
+      </c>
+      <c r="F210" s="14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="209" spans="3:6">
-      <c r="C209" s="14" t="s">
+    <row r="211" spans="2:6">
+      <c r="C211" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D209" s="14" t="s">
+      <c r="D211" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="E209" s="14">
+      <c r="E211" s="14">
         <v>8</v>
       </c>
-      <c r="F209" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="210" spans="3:6">
-      <c r="C210" s="14" t="s">
+      <c r="F211" s="14" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="212" spans="2:6">
+      <c r="C212" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D210" s="14" t="s">
+      <c r="D212" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="E210" s="14">
+      <c r="E212" s="14">
         <v>2</v>
       </c>
-      <c r="F210" s="14" t="s">
-        <v>241</v>
+      <c r="F212" s="14" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>